<commit_message>
Applied cases from reference paper without line segmentation
</commit_message>
<xml_diff>
--- a/Generator.xlsx
+++ b/Generator.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Number of Bus</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Name of Bus</t>
   </si>
   <si>
+    <t>MVA Base</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -52,25 +55,64 @@
     <t>APLAYA</t>
   </si>
   <si>
+    <t>104</t>
+  </si>
+  <si>
     <t>TAGALOAN</t>
   </si>
   <si>
+    <t>218</t>
+  </si>
+  <si>
     <t>PULANGUI 4</t>
   </si>
   <si>
+    <t>267</t>
+  </si>
+  <si>
     <t>DAVAO</t>
   </si>
   <si>
+    <t>32</t>
+  </si>
+  <si>
     <t>KIDAPAWAN</t>
   </si>
   <si>
+    <t>116</t>
+  </si>
+  <si>
     <t>KLINAN</t>
   </si>
   <si>
+    <t>59</t>
+  </si>
+  <si>
     <t>BALO-I</t>
   </si>
   <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
     <t>SANGALI</t>
+  </si>
+  <si>
+    <t>119</t>
   </si>
 </sst>
 </file>
@@ -78,10 +120,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;₱&quot;* #,##0_-;\-&quot;₱&quot;* #,##0_-;_-&quot;₱&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -89,6 +131,43 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -107,20 +186,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -129,9 +194,77 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,97 +277,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -245,43 +287,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,139 +461,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,8 +484,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -459,17 +501,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,8 +562,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -559,130 +601,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1012,35 +1054,35 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I2" sqref="I2:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="12.4444444444444" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.77777777777778" customWidth="1"/>
-    <col min="4" max="4" width="5.66666666666667" customWidth="1"/>
-    <col min="5" max="5" width="3.77777777777778" customWidth="1"/>
-    <col min="6" max="6" width="5.66666666666667" customWidth="1"/>
-    <col min="7" max="7" width="3.77777777777778" customWidth="1"/>
-    <col min="8" max="8" width="5.66666666666667" customWidth="1"/>
-    <col min="9" max="9" width="3" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.77777777777778" customWidth="1"/>
-    <col min="11" max="11" width="3.66666666666667" customWidth="1"/>
+    <col min="2" max="3" width="12.4444444444444" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.77777777777778" customWidth="1"/>
+    <col min="5" max="5" width="5.66666666666667" customWidth="1"/>
+    <col min="6" max="6" width="3.77777777777778" customWidth="1"/>
+    <col min="7" max="7" width="5.66666666666667" customWidth="1"/>
+    <col min="8" max="8" width="3.77777777777778" customWidth="1"/>
+    <col min="9" max="9" width="5.66666666666667" customWidth="1"/>
+    <col min="10" max="10" width="3" style="1" customWidth="1"/>
+    <col min="11" max="11" width="3.77777777777778" customWidth="1"/>
+    <col min="12" max="12" width="3.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1058,503 +1100,590 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D2">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>0.18*C2/100</f>
+        <v>0.1872</v>
       </c>
       <c r="F2">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <f>0.18*C2/100</f>
+        <v>0.1872</v>
       </c>
       <c r="H2">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I2">
+        <f>0.18*C2/100</f>
+        <v>0.1872</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
         <v>0</v>
       </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <f t="shared" ref="E3:E15" si="0">0.18*C3/100</f>
+        <v>0.1872</v>
       </c>
       <c r="F3">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <f t="shared" ref="G3:G15" si="1">0.18*C3/100</f>
+        <v>0.1872</v>
       </c>
       <c r="H3">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I3">
+        <f t="shared" ref="I3:I15" si="2">0.18*C3/100</f>
+        <v>0.1872</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
         <v>0</v>
       </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3924</v>
       </c>
       <c r="F4">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3924</v>
       </c>
       <c r="H4">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I4">
+        <f t="shared" si="2"/>
+        <v>0.3924</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.4806</v>
       </c>
       <c r="F5">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.4806</v>
       </c>
       <c r="H5">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0.4806</v>
+      </c>
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
         <v>0</v>
       </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D6">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.0576</v>
       </c>
       <c r="F6">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.0576</v>
       </c>
       <c r="H6">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0.0576</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.2088</v>
       </c>
       <c r="F7">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.2088</v>
       </c>
       <c r="H7">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0.2088</v>
+      </c>
+      <c r="J7">
         <v>1</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
         <v>0</v>
       </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D8">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.1062</v>
       </c>
       <c r="F8">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.1062</v>
       </c>
       <c r="H8">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0.1062</v>
+      </c>
+      <c r="J8">
         <v>1</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
         <v>0</v>
       </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D9">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.153</v>
       </c>
       <c r="F9">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.153</v>
       </c>
       <c r="H9">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0.153</v>
+      </c>
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
       <c r="K9">
         <v>0</v>
       </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3276</v>
       </c>
       <c r="F10">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3276</v>
       </c>
       <c r="H10">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I10">
+        <f t="shared" si="2"/>
+        <v>0.3276</v>
+      </c>
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
       <c r="K10">
         <v>0</v>
       </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D11">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.2988</v>
       </c>
       <c r="F11">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.2988</v>
       </c>
       <c r="H11">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0.2988</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
       <c r="K11">
         <v>0</v>
       </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.1026</v>
       </c>
       <c r="F12">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.1026</v>
       </c>
       <c r="H12">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0.1026</v>
+      </c>
+      <c r="J12">
         <v>1</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
         <v>0</v>
       </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D13">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.3762</v>
       </c>
       <c r="F13">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.3762</v>
       </c>
       <c r="H13">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0.3762</v>
+      </c>
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
       <c r="K13">
         <v>0</v>
       </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D14">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.2052</v>
       </c>
       <c r="F14">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.2052</v>
       </c>
       <c r="H14">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0.2052</v>
+      </c>
+      <c r="J14">
         <v>1</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
       <c r="K14">
         <v>0</v>
       </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D15">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.2142</v>
       </c>
       <c r="F15">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.2142</v>
       </c>
       <c r="H15">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0.2142</v>
+      </c>
+      <c r="J15">
         <v>1</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>0</v>
       </c>
     </row>

</xml_diff>